<commit_message>
updated dataset, collegeids sheet
</commit_message>
<xml_diff>
--- a/unitids.xlsx
+++ b/unitids.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdian\OneDrive\Documents\R\ClimateDataProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24F8335-C3DA-4D98-9A90-63A50888C545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D6BC4-D493-4D88-91D1-3834088E4F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UNIQUE COLLEGES" sheetId="1" r:id="rId1"/>
+    <sheet name="colleges and unit id's" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UNIQUE COLLEGES'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'colleges and unit id''s'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>college_name</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Western Washington University</t>
-  </si>
-  <si>
-    <t>SUNY University at Buffalo</t>
   </si>
   <si>
     <t>Texas A&amp;M University System</t>
@@ -203,7 +200,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,12 +232,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,382 +552,373 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D0CF5A-9825-4CB5-9F05-DAB46EBF540D}">
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="44.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>131159</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>104151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>164988</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>211440</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>190099</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>126818</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>190150</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>212054</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>131469</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>131496</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>167358</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>147767</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>204857</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>195003</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>179159</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>149231</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>243744</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3">
+        <v>196413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3">
+        <v>228547</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3">
+        <v>216339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3">
+        <v>131283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3">
+        <v>204796</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="4">
         <v>196088</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4">
-        <v>196413</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="4">
-        <v>228547</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="4">
-        <v>216339</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4">
-        <v>131283</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="4">
-        <v>204796</v>
-      </c>
-    </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3"/>
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3">
+        <v>110635</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4">
-        <v>110635</v>
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3">
+        <v>145637</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="4">
-        <v>145637</v>
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3">
+        <v>163286</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="4">
-        <v>163286</v>
+      <c r="A32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3">
+        <v>174066</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="4">
-        <v>174066</v>
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="3">
+        <v>178396</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="4">
-        <v>178396</v>
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>183044</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="4">
-        <v>183044</v>
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
+        <v>227216</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="4">
-        <v>227216</v>
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3">
+        <v>207500</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="4">
-        <v>207500</v>
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="3">
+        <v>215062</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4">
-        <v>215062</v>
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3">
+        <v>215293</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="4">
-        <v>215293</v>
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="3">
+        <v>137351</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="4">
-        <v>137351</v>
+      <c r="A40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="3">
+        <v>221759</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="4">
-        <v>221759</v>
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3">
+        <v>230764</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="4">
-        <v>230764</v>
+      <c r="A42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3">
+        <v>231174</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="4">
-        <v>231174</v>
+      <c r="A43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3">
+        <v>234076</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="4">
-        <v>234076</v>
+      <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="3">
+        <v>240444</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="4">
-        <v>240444</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B45" s="3">
         <v>237011</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A46">
-    <sortCondition ref="A8:A46"/>
-  </sortState>
+  <autoFilter ref="A1:B1" xr:uid="{52D0CF5A-9825-4CB5-9F05-DAB46EBF540D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>